<commit_message>
Update NAFTA green button code
</commit_message>
<xml_diff>
--- a/GreenButton/HarmanPana All Networks/NAFTA/Bench Config - Green Button v1.xlsx
+++ b/GreenButton/HarmanPana All Networks/NAFTA/Bench Config - Green Button v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theul_000\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\New-CANBoard-Code-master-PNET\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Bench Configuration</t>
   </si>
@@ -56,9 +56,6 @@
     <t>VR</t>
   </si>
   <si>
-    <t>Mute</t>
-  </si>
-  <si>
     <t>Off</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t>ENG. Mode</t>
   </si>
   <si>
-    <t>Door Ajar</t>
-  </si>
-  <si>
     <t>Vol Down</t>
   </si>
   <si>
@@ -116,19 +110,28 @@
     <t>Dealer Mode</t>
   </si>
   <si>
-    <t>Assist</t>
-  </si>
-  <si>
-    <t>Theft Alarm</t>
-  </si>
-  <si>
     <t>CUSW - UF</t>
   </si>
   <si>
-    <t>1C3ADECZ7GV1002UC</t>
-  </si>
-  <si>
     <t>MY16 - UF</t>
+  </si>
+  <si>
+    <t>1C3CCCCB7FN1124UC</t>
+  </si>
+  <si>
+    <t>Radio Off</t>
+  </si>
+  <si>
+    <t>Night Mode</t>
+  </si>
+  <si>
+    <t>Day Mode</t>
+  </si>
+  <si>
+    <t>Phone Pickup Long Press</t>
+  </si>
+  <si>
+    <t>VR Long Press</t>
   </si>
 </sst>
 </file>
@@ -177,11 +180,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,9 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -476,77 +477,77 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5546875" customWidth="1"/>
-    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>5</v>
@@ -564,68 +565,68 @@
         <v>9</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="L6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="1">
-        <v>911</v>
+      <c r="N6" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="L7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="M7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="N7" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -633,10 +634,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -644,10 +645,10 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -655,10 +656,10 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <v>6</v>

</xml_diff>